<commit_message>
added callbacks and functions
</commit_message>
<xml_diff>
--- a/data/lab4_drug-description.xlsx
+++ b/data/lab4_drug-description.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apitt\Documents\UBC\MDS\532_DS_viz2\DSCI_532_Group_113_Overdose\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apitt\Documents\UBC\MDS\532_DS_viz2\DSCI_532_Group_113_Overdose_R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D80CE25-41B1-4398-9591-8D4E8225C27F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A80060-C199-46D4-9050-C4319BF6C26A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2200C2C8-EF8B-4EAE-95C9-AE9F1803E73F}"/>
   </bookViews>
@@ -199,9 +199,6 @@
     <t>https://www.drugbank.ca/structures/DB00193/thumb.svg</t>
   </si>
   <si>
-    <t>Hydrocone</t>
-  </si>
-  <si>
     <r>
       <t>Hydrocodone is a synthetic opioid derivative of codeine. It is commonly used in combination with </t>
     </r>
@@ -487,6 +484,9 @@
   </si>
   <si>
     <t>https://www.drugbank.ca/assets/logo-pink-bd7264e3b993f48d681445728e394507ac912eb6e426e52c6d3230a78dae4bc6.svg</t>
+  </si>
+  <si>
+    <t>Hydrocodone</t>
   </si>
 </sst>
 </file>
@@ -876,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{957C0A05-3243-4389-AFB0-D9459F1B2568}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -893,7 +893,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -907,7 +907,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
@@ -921,7 +921,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -935,7 +935,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -949,7 +949,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -963,7 +963,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -977,7 +977,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -991,7 +991,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1005,7 +1005,7 @@
         <v>24</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1019,74 +1019,74 @@
         <v>28</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>